<commit_message>
Pushin it to the limit
send help
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutta\Documents\GitHub\nationwidehackathon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexa\OneDrive\Documents\GitHub\nationwidehackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A83F76-A431-4597-9FB9-BB69E9AFB333}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{F8A83F76-A431-4597-9FB9-BB69E9AFB333}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{1C4A43E4-CA35-42BF-A7CB-B5AB4BE3B124}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13149" windowHeight="3626" xr2:uid="{4E487CA1-ADF2-4C76-8CE1-AED505A0E441}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13155" windowHeight="3630" xr2:uid="{4E487CA1-ADF2-4C76-8CE1-AED505A0E441}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,1212 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7500000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9680000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>132600000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88400000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A7C6-4C78-BC47-0444966D0BDB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="505738432"/>
+        <c:axId val="505742040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="505738432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="505742040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="505742040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="505738432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7500000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$1:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1100000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2700000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1300000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3400000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9A5C-49EB-A89F-BFBAB4EE73B6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="321562096"/>
+        <c:axId val="321559144"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="321562096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="321559144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="321559144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="321562096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7500000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$1:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4853952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26222435</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5506839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5067804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3792199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-07EA-4CB1-9CD5-A4788AE347D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="607455000"/>
+        <c:axId val="607452048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="607455000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="607452048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="607452048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="607455000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1028,6 +2233,1554 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1061,6 +3814,114 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FC3DC28-B65F-4EA0-BB02-F09941B36B99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>52387</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F39BAF3-A390-4124-A6FD-4EF39C4BD712}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>528637</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDF9C3BA-DD9C-401C-AF33-B5257827CE30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1369,19 +4230,19 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="9.23046875" style="1"/>
-    <col min="9" max="9" width="8.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="23.69140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.23046875" style="1"/>
+    <col min="1" max="8" width="9.28515625" style="1"/>
+    <col min="9" max="9" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>25</v>
       </c>
@@ -1420,7 +4281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42</v>
       </c>
@@ -1459,7 +4320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>35</v>
       </c>
@@ -1498,7 +4359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>54</v>
       </c>
@@ -1537,7 +4398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>72</v>
       </c>
@@ -1576,12 +4437,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J6" s="1">
+        <v>140940835</v>
+      </c>
+      <c r="K6" s="1">
+        <f>40000000 * 2.718^(0.00000000007 * J6)</f>
+        <v>40396546.136011347</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16.3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
         <v>3</v>
       </c>

</xml_diff>